<commit_message>
updated date case classes to hold different date formats and lexicon is updated accordingly.
</commit_message>
<xml_diff>
--- a/src/main/docs/Queries_CCG_Derivation.xlsx
+++ b/src/main/docs/Queries_CCG_Derivation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="187">
   <si>
     <t xml:space="preserve">events</t>
   </si>
@@ -135,6 +135,9 @@
     <t xml:space="preserve">happening</t>
   </si>
   <si>
+    <t xml:space="preserve">related</t>
+  </si>
+  <si>
     <t xml:space="preserve">that </t>
   </si>
   <si>
@@ -144,136 +147,37 @@
     <t xml:space="preserve">part of</t>
   </si>
   <si>
-    <t xml:space="preserve">Filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tasks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuzzy Search string – Subject , Tags</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are all the tasks assigned to me ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are all the events that I am participating ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are all the tasks assigned by me ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all the events that I am participating / I am a speaker / Created by me / I am organizing/ volunteering?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speaker/Creater/Organizer/Volunteer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Events I am a participant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Events organized by me</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oganizer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participating/organizing/speaking events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are all the tasks that are overdue?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what are all the events happening near to me ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are all the overdue tasks?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all the events that  I am a speaking ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">near location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overdue tasks?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Events happening today?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is task #353179?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Events scheduled for vaishnavi by onboarding manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task#353179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">my events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speaker Or Creater Or Organizer Or Volunteer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the planned date of task#353179?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">recent training in java</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Training</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the planned start date of task#353179?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schedule event for new joiner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there any issues assigned with the tasks?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">who is the SPOC for Java training in India to vaishnavi?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tasks assigned.</t>
+    <t xml:space="preserve">NP/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">organized </t>
+  </si>
+  <si>
+    <t xml:space="preserve">by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S/NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NP\V)/NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP\V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP\(NP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">between</t>
   </si>
   <si>
     <r>
@@ -283,7 +187,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">List all the Java related events between 1</t>
+      <t xml:space="preserve">1</t>
     </r>
     <r>
       <rPr>
@@ -302,7 +206,21 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> of March to 4</t>
+      <t xml:space="preserve"> of March</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">and </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
     </r>
     <r>
       <rPr>
@@ -312,7 +230,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">th</t>
+      <t xml:space="preserve">nd</t>
     </r>
     <r>
       <rPr>
@@ -321,11 +239,155 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> of March.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">JAVA</t>
+      <t xml:space="preserve"> of March</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">(S\NP)/NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (NP\NP)/NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NP\NP)/NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NP\NP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(S\NP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuzzy Search string – Subject , Tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are all the tasks assigned to me ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are all the events that I am participating ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are all the tasks assigned by me ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all the events that I am participating / I am a speaker / Created by me / I am organizing/ volunteering?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaker/Creater/Organizer/Volunteer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Events I am a participant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Events organized by me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oganizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participating/organizing/speaking events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are all the tasks that are overdue?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what are all the events happening near me ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are all the overdue tasks?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all the events that  I am a speaking ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">near location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overdue tasks?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Events happening today?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is task #353179?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Events scheduled for vaishnavi by onboarding manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task#353179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">my events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaker Or Creater Or Organizer Or Volunteer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the planned date of task#353179?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recent training in java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the planned start date of task#353179?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schedule event for new joiner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there any issues assigned with the tasks?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who is the SPOC for Java training in India to vaishnavi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tasks assigned.</t>
   </si>
   <si>
     <r>
@@ -333,8 +395,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">List all the Java related events between 1</t>
     </r>
     <r>
       <rPr>
@@ -342,6 +405,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -350,18 +414,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> March </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">4</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> of March and 4</t>
     </r>
     <r>
       <rPr>
@@ -369,6 +424,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -377,123 +433,13 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> March</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">assigned tasks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List all the Java related events happening this week.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current week start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current week End</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When is the next celebration scheduled ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not sure these are related to events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tasks overdue?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When is the next birthday celebration ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efforts spent on the task#1234?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Who is celebrating the next birthday?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efforts spent on task#1234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what are all the cultural / work anniversary events scheduled this month?. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cultural / Work Anniversary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Month Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Month End</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is there any risks assigned with the tasks?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oracle workshops in chennai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workshop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of tasks pending for me ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what are all the meetings I have today ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">me</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of tasks that are open / In-progress / Closed ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What time I am free today?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open tasks?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what are all the upcoming events this week?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tommorow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end of week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task criticality wise status ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Who is having the next birthday?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categories of open task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Whose birthday is coming up?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task that require my immediate attention?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What are all the recommended events for me ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My recommendation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of all my tasks?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">recommended events ?.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">List 5 tasks?</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> of March.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">JAVA</t>
   </si>
   <si>
     <r>
@@ -503,7 +449,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">List all the upcoming account / project activities between 15</t>
+      <t xml:space="preserve">1</t>
     </r>
     <r>
       <rPr>
@@ -513,7 +459,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">th</t>
+      <t xml:space="preserve">st</t>
     </r>
     <r>
       <rPr>
@@ -522,7 +468,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> march to 14</t>
+      <t xml:space="preserve"> March </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
     </r>
     <r>
       <rPr>
@@ -541,11 +498,119 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> April ?</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">account/Project</t>
+      <t xml:space="preserve"> March</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">assigned tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List all the Java related events happening this week.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current week start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current week End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When is the next celebration scheduled ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not sure these are related to events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tasks overdue?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When is the next birthday celebration ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efforts spent on the task#1234?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who is celebrating the next birthday?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efforts spent on task#1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what are all the cultural / work anniversary events scheduled this month?. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cultural / Work Anniversary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there any risks assigned with the tasks?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle workshops in chennai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of tasks pending for me ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what are all the meetings I have today ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of tasks that are open / In-progress / Closed ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What time I am free today?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open tasks?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what are all the upcoming events this week?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommorow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end of week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task criticality wise status ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Who is having the next birthday?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categories of open task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whose birthday is coming up?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task that require my immediate attention?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are all the recommended events for me ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My recommendation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status of all my tasks?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recommended events ?.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List 5 tasks?</t>
   </si>
   <si>
     <r>
@@ -553,8 +618,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">15</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">List all the upcoming account / project activities between 15</t>
     </r>
     <r>
       <rPr>
@@ -562,6 +628,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -570,18 +637,9 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> March</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">14</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> march to 14</t>
     </r>
     <r>
       <rPr>
@@ -589,6 +647,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -597,12 +656,79 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> April ?</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">account/Project</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">15</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> March</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">14</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> April</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">task count by category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list all the events in chennai</t>
   </si>
   <si>
     <t xml:space="preserve">List the top players completed the tasks?</t>
@@ -650,6 +776,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -659,6 +786,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -669,6 +797,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -678,6 +807,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -687,6 +817,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"assigned"</t>
     </r>
@@ -696,6 +827,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)-&gt; </t>
     </r>
@@ -706,6 +838,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">relation</t>
     </r>
@@ -715,6 +848,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -724,6 +858,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"b"</t>
     </r>
@@ -733,6 +868,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)) +
   (</t>
@@ -744,6 +880,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -753,6 +890,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -762,6 +900,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"who"</t>
     </r>
@@ -771,6 +910,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -780,6 +920,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"what"</t>
     </r>
@@ -789,6 +930,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -798,6 +940,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"how"</t>
     </r>
@@ -807,6 +950,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -816,6 +960,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"where"</t>
     </r>
@@ -825,6 +970,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -834,6 +980,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"when"</t>
     </r>
@@ -843,6 +990,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">) -&gt; Q) +
   (</t>
@@ -854,6 +1002,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -863,6 +1012,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -872,6 +1022,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"tasks"</t>
     </r>
@@ -881,6 +1032,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">) -&gt; T) +
   (</t>
@@ -892,6 +1044,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -901,6 +1054,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -910,6 +1064,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"are"</t>
     </r>
@@ -919,6 +1074,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)-&gt;(((NP\Q)/NP)</t>
     </r>
@@ -928,6 +1084,7 @@
         <color rgb="FF808080"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/*,λ {pred: String =&gt;λ{pre:String =&gt; Query(pred,pre)}}*/</t>
     </r>
@@ -937,6 +1094,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)) +
   (</t>
@@ -948,6 +1106,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -957,6 +1116,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -966,6 +1126,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"all"</t>
     </r>
@@ -975,6 +1136,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)-&gt;((NP/NP))) +
   (</t>
@@ -986,6 +1148,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -995,6 +1158,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -1004,6 +1168,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"the"</t>
     </r>
@@ -1013,6 +1178,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)-&gt;</t>
     </r>
@@ -1023,6 +1189,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -1032,6 +1199,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">((NP/NP)</t>
     </r>
@@ -1041,6 +1209,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,</t>
     </r>
@@ -1050,6 +1219,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(NP/T))) +
   (</t>
@@ -1061,6 +1231,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -1070,6 +1241,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -1079,6 +1251,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"to"</t>
     </r>
@@ -1088,6 +1261,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,</t>
     </r>
@@ -1097,6 +1271,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"by"</t>
     </r>
@@ -1106,6 +1281,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)-&gt;(NP/NP)) +
   (</t>
@@ -1117,6 +1293,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -1126,6 +1303,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -1135,6 +1313,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"me"</t>
     </r>
@@ -1144,6 +1323,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)-&gt;(NP)) +
   (</t>
@@ -1155,6 +1335,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -1164,6 +1345,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -1173,6 +1355,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"overdue"</t>
     </r>
@@ -1182,6 +1365,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)-&gt;((NP/T)</t>
     </r>
@@ -1191,6 +1375,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,</t>
     </r>
@@ -1201,6 +1386,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="DejaVu Sans Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">λ</t>
     </r>
@@ -1210,6 +1396,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{pre:</t>
     </r>
@@ -1219,6 +1406,7 @@
         <color rgb="FF4E807D"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">String </t>
     </r>
@@ -1228,6 +1416,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">=&gt; </t>
     </r>
@@ -1238,6 +1427,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Query</t>
     </r>
@@ -1247,6 +1437,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -1256,6 +1447,7 @@
         <color rgb="FF6A8759"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">"test"</t>
     </r>
@@ -1265,6 +1457,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,</t>
     </r>
@@ -1274,6 +1467,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">pre)})) +
   </t>
@@ -1284,6 +1478,7 @@
         <color rgb="FF808080"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">//(Seq("are")-&gt;((((S\Q)\NP)\NP)/NP, λ {pred: String =&gt;λ{ pre:String=&gt;λ{ check:String=&gt;λ {subject: String =&gt; Define(check+pre, subject, pred)}}}}))+
   /*(Seq("many") -&gt; (NP)) +
@@ -1297,6 +1492,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(Else -&gt; </t>
     </r>
@@ -1307,6 +1503,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -1316,6 +1513,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(N % </t>
     </r>
@@ -1325,6 +1523,7 @@
         <color rgb="FF6897BB"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0.8</t>
     </r>
@@ -1334,6 +1533,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -1343,6 +1543,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">N/N % </t>
     </r>
@@ -1352,6 +1553,7 @@
         <color rgb="FF6897BB"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0.1</t>
     </r>
@@ -1361,6 +1563,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -1370,6 +1573,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">X % </t>
     </r>
@@ -1379,6 +1583,7 @@
         <color rgb="FF6897BB"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0.1</t>
     </r>
@@ -1388,6 +1593,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">))
 </t>
@@ -1399,6 +1605,7 @@
         <color rgb="FFCC7832"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">private def </t>
     </r>
@@ -1408,6 +1615,7 @@
         <color rgb="FFFFC66D"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">relation</t>
     </r>
@@ -1417,6 +1625,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(relationType: </t>
     </r>
@@ -1426,6 +1635,7 @@
         <color rgb="FF4E807D"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">String</t>
     </r>
@@ -1435,6 +1645,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">) = {
   </t>
@@ -1446,6 +1657,7 @@
         <color rgb="FF9876AA"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Seq</t>
     </r>
@@ -1455,6 +1667,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(
     </t>
@@ -1465,6 +1678,7 @@
         <color rgb="FF808080"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">// e.g. "Checkers is a dog"
     </t>
@@ -1475,6 +1689,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">((NP\T)/NP</t>
     </r>
@@ -1484,6 +1699,7 @@
         <color rgb="FF808080"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/*,λ{pre:String =&gt; Query("pred",pre)}*/</t>
     </r>
@@ -1493,6 +1709,7 @@
         <color rgb="FFA9B7C6"/>
         <rFont val="Source Code Pro"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)
   )
@@ -1546,12 +1763,6 @@
   </si>
   <si>
     <t xml:space="preserve">task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(S\NP)/NP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(S\NP)</t>
   </si>
   <si>
     <t xml:space="preserve">((S\NP)\NP)/NP</t>
@@ -1582,11 +1793,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1604,7 +1816,18 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
+      <sz val="10.5"/>
+      <name val="Source Code Pro"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1617,35 +1840,18 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10.5"/>
       <color rgb="FFA9B7C6"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FFA9B7C6"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -1653,12 +1859,14 @@
       <color rgb="FF9876AA"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FF6A8759"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -1666,18 +1874,21 @@
       <color rgb="FFA9B7C6"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FFCC7832"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FF808080"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -1685,18 +1896,21 @@
       <color rgb="FFA9B7C6"/>
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FF4E807D"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FF6897BB"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1704,15 +1918,17 @@
       <color rgb="FFCC7832"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FFFFC66D"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1729,6 +1945,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFCC7832"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33FF99"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1779,7 +2007,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1816,27 +2044,55 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1844,7 +2100,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1888,7 +2144,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFCC7832"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
@@ -1908,11 +2164,11 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFC66D"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF33FF99"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFCC7832"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF9876AA"/>
       <rgbColor rgb="FF003366"/>
@@ -1941,7 +2197,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1959,17 +2215,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:P71"/>
+  <dimension ref="B2:P110"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C110" activeCellId="0" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,81 +2695,438 @@
       <c r="E53" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="0" t="s">
+      <c r="F56" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="0" t="s">
+      <c r="B57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F57" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="1" t="s">
+      <c r="F57" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="7"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="9"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="10"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F70" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G69" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="H70" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I69" s="1" t="s">
+      <c r="I70" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="5" t="s">
+      <c r="J70" s="9"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="C72" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="D72" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="E72" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="4"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="12"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D87" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C88" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D94" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C95" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" s="9"/>
+    </row>
+    <row r="99" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" s="13"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I102" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C103" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H103" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I103" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H105" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I105" s="14"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G106" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H106" s="15"/>
+      <c r="I106" s="15"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F107" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G107" s="16"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E108" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F108" s="16"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="16"/>
+      <c r="I108" s="16"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D109" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E109" s="16"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="16"/>
+      <c r="I109" s="16"/>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C110" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" s="16"/>
+      <c r="E110" s="16"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="16"/>
+      <c r="I110" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="43">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:E7"/>
@@ -2534,10 +3149,31 @@
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="B89:E89"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="G106:I106"/>
+    <mergeCell ref="F107:I107"/>
+    <mergeCell ref="E108:I108"/>
+    <mergeCell ref="D109:I109"/>
+    <mergeCell ref="C110:I110"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2553,573 +3189,576 @@
   <dimension ref="B1:N40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="88.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="9" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="9" width="40.0459183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="9" width="14.3979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="9" width="18.5663265306122"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="9" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="87.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="17" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="17" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="17" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="17" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="10"/>
-      <c r="D1" s="11"/>
-      <c r="G1" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="G1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>49</v>
+      <c r="F2" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="10"/>
+      <c r="B3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="9" t="s">
+      <c r="I4" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="9" t="s">
+      <c r="I5" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="9" t="s">
+      <c r="D6" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>53</v>
+      <c r="I6" s="17" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="9" t="s">
+      <c r="D7" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>59</v>
+      <c r="I7" s="17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="9" t="s">
+      <c r="I8" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>56</v>
+      <c r="I9" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>66</v>
+      <c r="I10" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>69</v>
+      <c r="L11" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="9" t="s">
-        <v>74</v>
+      <c r="I13" s="17" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>77</v>
+        <v>96</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="L17" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>86</v>
+      <c r="H17" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>90</v>
+      <c r="H18" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>92</v>
+        <v>87</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="15"/>
+        <v>113</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="22"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="15"/>
+        <v>115</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="L22" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>101</v>
+        <v>118</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="L22" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="M22" s="17" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="N23" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="N23" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="L24" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>69</v>
+        <v>126</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M24" s="17" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>110</v>
+        <v>128</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="M26" s="9" t="s">
-        <v>114</v>
+      <c r="L26" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="M26" s="17" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>116</v>
+        <v>134</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>118</v>
+        <v>136</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K29" s="9" t="s">
-        <v>121</v>
+      <c r="K29" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G30" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="9" t="s">
-        <v>121</v>
+      <c r="K30" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G31" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="L31" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="M31" s="9" t="s">
-        <v>128</v>
+      <c r="J31" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="M31" s="17" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>129</v>
+        <v>148</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="6" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="0" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D39" s="0" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="0" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3129,7 +3768,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3150,18 +3789,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="259.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="16" t="s">
-        <v>143</v>
+      <c r="D5" s="23" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3182,12 +3821,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3208,52 +3847,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
+      <c r="F2" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>28</v>
@@ -3262,10 +3901,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>28</v>
@@ -3292,7 +3931,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="7" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -3326,7 +3965,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="7" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -3348,37 +3987,37 @@
       <c r="I11" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>145</v>
+      <c r="F16" s="25" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>148</v>
+      <c r="C17" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3396,7 +4035,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="3" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -3412,38 +4051,38 @@
       <c r="F22" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>108</v>
+      <c r="B27" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="B28" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="7" t="s">
@@ -3453,7 +4092,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="7" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -3467,23 +4106,23 @@
       <c r="E32" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>145</v>
+      <c r="F36" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3491,7 +4130,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>28</v>
@@ -3500,10 +4139,10 @@
         <v>28</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3529,7 +4168,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="3" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -3547,20 +4186,20 @@
       <c r="G43" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="E49" s="18" t="s">
+      <c r="B49" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="C49" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="E49" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="18" t="s">
-        <v>159</v>
+      <c r="F49" s="25" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3568,16 +4207,16 @@
         <v>4</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>160</v>
+        <v>54</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3595,7 +4234,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="3" t="s">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -3611,29 +4250,29 @@
       <c r="F55" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="18" t="s">
+      <c r="B58" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="18" t="s">
+      <c r="D58" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E58" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="G58" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="H58" s="18" t="s">
+      <c r="E58" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="F58" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="G58" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="H58" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I58" s="18" t="s">
-        <v>159</v>
+      <c r="I58" s="25" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3646,20 +4285,20 @@
       <c r="D59" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E59" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="G59" s="9" t="s">
+      <c r="E59" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="G59" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H59" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="I59" s="9" t="s">
-        <v>149</v>
+      <c r="H59" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="I59" s="17" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3677,7 +4316,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F62" s="3" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -3685,7 +4324,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="3" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -3718,64 +4357,64 @@
       <c r="I66" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="18" t="s">
+      <c r="C69" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="E69" s="18" t="s">
+      <c r="D69" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="E69" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F69" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="G69" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="H69" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="I69" s="18" t="s">
-        <v>108</v>
+      <c r="F69" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="G69" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="H69" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="I69" s="25" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="9" t="s">
+      <c r="C70" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D70" s="9" t="s">
+      <c r="D70" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="E70" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F70" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G70" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="H70" s="9" t="s">
+      <c r="F70" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="H70" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I70" s="9" t="s">
+      <c r="I70" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9"/>
-      <c r="G71" s="9"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+      <c r="G71" s="17"/>
       <c r="H71" s="3" t="s">
         <v>4</v>
       </c>
@@ -3787,7 +4426,7 @@
       </c>
       <c r="C72" s="3"/>
       <c r="G72" s="3" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -3799,7 +4438,7 @@
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="F73" s="3" t="s">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
@@ -3826,31 +4465,31 @@
       <c r="I75" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="C79" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="E79" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F79" s="18" t="s">
-        <v>145</v>
+      <c r="B79" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C79" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="E79" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="F79" s="25" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="5" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3907,7 +4546,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
updated lexicon to handle few more queries
</commit_message>
<xml_diff>
--- a/src/main/docs/Queries_CCG_Derivation.xlsx
+++ b/src/main/docs/Queries_CCG_Derivation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="192">
   <si>
     <t xml:space="preserve">events</t>
   </si>
@@ -256,6 +256,24 @@
   </si>
   <si>
     <t xml:space="preserve">(S\NP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP/I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S\NP</t>
   </si>
   <si>
     <t xml:space="preserve">Filter</t>
@@ -1769,9 +1787,6 @@
   </si>
   <si>
     <t xml:space="preserve">(S\NP)\NP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S\NP</t>
   </si>
   <si>
     <t xml:space="preserve">(S\NP)\T)/NP</t>
@@ -1943,14 +1958,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFD9D9D9"/>
+        <fgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFCC7832"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
-        <bgColor rgb="FFCC7832"/>
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
     <fill>
@@ -2007,8 +2022,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2016,11 +2035,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2028,23 +2063,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2052,7 +2071,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2084,11 +2111,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2104,11 +2135,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2215,10 +2246,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:P110"/>
+  <dimension ref="B2:P148"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C110" activeCellId="0" sqref="C110"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A123" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B143" activeCellId="0" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2230,21 +2261,21 @@
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2258,20 +2289,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -2279,18 +2311,20 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
@@ -2301,47 +2335,50 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
@@ -2367,7 +2404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -2377,7 +2414,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
         <v>4</v>
       </c>
@@ -2389,7 +2426,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
@@ -2401,7 +2438,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
@@ -2413,7 +2450,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
@@ -2425,54 +2462,56 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="1" t="s">
+    <row r="24" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="K26" s="2" t="s">
         <v>22</v>
       </c>
       <c r="L26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="M26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="N26" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="O26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P26" s="1" t="s">
+      <c r="P26" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
@@ -2492,7 +2531,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -2500,51 +2539,53 @@
       <c r="F28" s="5"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="7"/>
+    <row r="29" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="3"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="7" t="s">
+    <row r="30" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="7" t="s">
+    <row r="31" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="1" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="2" t="s">
         <v>4</v>
       </c>
@@ -2564,103 +2605,104 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="7"/>
+    <row r="36" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="7" t="s">
+    <row r="38" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="7" t="s">
+    <row r="39" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G40" s="7"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="7" t="s">
+      <c r="F40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="7"/>
+      <c r="B46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C49" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2671,318 +2713,318 @@
       <c r="E50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
+      <c r="B51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="4"/>
+      <c r="B52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
+      <c r="B53" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H56" s="9"/>
+      <c r="H56" s="10"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="C57" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E58" s="2"/>
+      <c r="E58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
+      <c r="B59" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
+      <c r="B60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="4"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="9"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G65" s="1" t="s">
+      <c r="G65" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H65" s="9"/>
+      <c r="H65" s="10"/>
     </row>
     <row r="66" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="10"/>
+      <c r="C66" s="11"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F70" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="G70" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="H70" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I70" s="1" t="s">
+      <c r="I70" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J70" s="9"/>
+      <c r="J70" s="10"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E72" s="12" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F77" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="2" t="s">
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="9"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
+      <c r="B81" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="12"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
+      <c r="B82" s="15"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D85" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="E85" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D87" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E87" s="3"/>
+      <c r="D87" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" s="14"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
+      <c r="C88" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D91" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D92" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E92" s="2" t="s">
+      <c r="E92" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E94" s="3"/>
+      <c r="E94" s="14"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
+      <c r="C95" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="0" t="s">
@@ -2997,7 +3039,7 @@
       <c r="E98" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F98" s="9"/>
+      <c r="F98" s="10"/>
     </row>
     <row r="99" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="0" t="s">
@@ -3006,7 +3048,7 @@
       <c r="C99" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D99" s="10" t="s">
+      <c r="D99" s="11" t="s">
         <v>49</v>
       </c>
       <c r="E99" s="0" t="s">
@@ -3014,34 +3056,34 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C100" s="13"/>
+      <c r="B100" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" s="16"/>
     </row>
     <row r="102" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E102" s="5" t="s">
+      <c r="E102" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F102" s="5" t="s">
+      <c r="F102" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G102" s="5" t="s">
+      <c r="G102" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H102" s="5" t="s">
+      <c r="H102" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I102" s="5" t="s">
+      <c r="I102" s="12" t="s">
         <v>53</v>
       </c>
     </row>
@@ -3049,84 +3091,300 @@
       <c r="C103" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E103" s="5" t="s">
+      <c r="E103" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F103" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="G103" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H103" s="5" t="s">
+      <c r="G103" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H103" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="I103" s="5" t="s">
+      <c r="I103" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
+      <c r="E104" s="12"/>
+      <c r="G104" s="12"/>
+      <c r="H104" s="12"/>
+      <c r="I104" s="12"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H105" s="14" t="s">
+      <c r="H105" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I105" s="14"/>
+      <c r="I105" s="17"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G106" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H106" s="15"/>
-      <c r="I106" s="15"/>
+      <c r="G106" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F107" s="16" t="s">
+      <c r="F107" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G107" s="16"/>
-      <c r="H107" s="16"/>
-      <c r="I107" s="16"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="19"/>
+      <c r="I107" s="19"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E108" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F108" s="16"/>
-      <c r="G108" s="16"/>
-      <c r="H108" s="16"/>
-      <c r="I108" s="16"/>
+      <c r="E108" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F108" s="19"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="19"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D109" s="16" t="s">
+      <c r="D109" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E109" s="16"/>
-      <c r="F109" s="16"/>
-      <c r="G109" s="16"/>
-      <c r="H109" s="16"/>
-      <c r="I109" s="16"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="19"/>
+      <c r="I109" s="19"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C110" s="16" t="s">
+      <c r="C110" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D110" s="16"/>
-      <c r="E110" s="16"/>
-      <c r="F110" s="16"/>
-      <c r="G110" s="16"/>
-      <c r="H110" s="16"/>
-      <c r="I110" s="16"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="19"/>
+      <c r="H110" s="19"/>
+      <c r="I110" s="19"/>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C117" s="3"/>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="7"/>
+      <c r="C123" s="12"/>
+      <c r="D123" s="12"/>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="12"/>
+      <c r="C124" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" s="3"/>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C131" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D131" s="3"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D135" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E135" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D137" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E137" s="3"/>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C138" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+      <c r="E139" s="3"/>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B142" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E143" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F143" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="7"/>
+      <c r="C144" s="12"/>
+      <c r="D144" s="12"/>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E145" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F145" s="19"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D146" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E146" s="19"/>
+      <c r="F146" s="19"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C147" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D147" s="19"/>
+      <c r="E147" s="19"/>
+      <c r="F147" s="19"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148" s="19"/>
+      <c r="D148" s="19"/>
+      <c r="E148" s="19"/>
+      <c r="F148" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="55">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:E7"/>
@@ -3170,6 +3428,18 @@
     <mergeCell ref="E108:I108"/>
     <mergeCell ref="D109:I109"/>
     <mergeCell ref="C110:I110"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="B125:D125"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="B132:D132"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="C138:E138"/>
+    <mergeCell ref="B139:E139"/>
+    <mergeCell ref="E145:F145"/>
+    <mergeCell ref="D146:F146"/>
+    <mergeCell ref="C147:F147"/>
+    <mergeCell ref="B148:F148"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3189,7 +3459,7 @@
   <dimension ref="B1:N40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3199,566 +3469,566 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="87.0714285714286"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="17" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="17" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="17" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="17" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="20" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="20" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="20" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="20" width="11.3418367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="G1" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="G1" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="B2" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="18" t="s">
+      <c r="F2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="G2" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="H2" s="21" t="s">
         <v>69</v>
       </c>
+      <c r="I2" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="18"/>
+      <c r="B3" s="21"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" s="17" t="s">
+      <c r="I4" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="K5" s="17" t="s">
+      <c r="I5" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="17" t="s">
+      <c r="D6" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>73</v>
+      <c r="I6" s="20" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>79</v>
+      <c r="I7" s="20" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="K8" s="17" t="s">
+      <c r="I8" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>82</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="N10" s="17" t="s">
-        <v>86</v>
+      <c r="I10" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>89</v>
+      <c r="L11" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="17" t="s">
-        <v>94</v>
+      <c r="I13" s="20" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>97</v>
+        <v>102</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="M17" s="17" t="s">
-        <v>106</v>
+      <c r="H17" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="L17" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="M17" s="20" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="L18" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="M18" s="17" t="s">
+      <c r="H18" s="20" t="s">
         <v>110</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="M18" s="20" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>112</v>
+        <v>93</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" s="22"/>
+        <v>119</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21" s="22"/>
+        <v>121</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="L22" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="M22" s="17" t="s">
-        <v>121</v>
+        <v>124</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="L22" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="M22" s="20" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="N23" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="N23" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="K24" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="K24" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="L24" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="M24" s="17" t="s">
-        <v>89</v>
+      <c r="L24" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>129</v>
+        <v>134</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L26" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="M26" s="17" t="s">
-        <v>133</v>
+      <c r="L26" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>135</v>
+        <v>140</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>137</v>
+        <v>142</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K29" s="17" t="s">
-        <v>140</v>
+      <c r="K29" s="20" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G30" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="17" t="s">
-        <v>140</v>
+      <c r="K30" s="20" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G31" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="L31" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="M31" s="17" t="s">
-        <v>147</v>
+      <c r="J31" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="L31" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="M31" s="20" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="6" t="s">
-        <v>150</v>
+      <c r="B33" s="24" t="s">
+        <v>156</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D39" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3793,8 +4063,8 @@
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="259.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="23" t="s">
-        <v>163</v>
+      <c r="D5" s="27" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3854,653 +4124,653 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="E2" s="24" t="s">
+      <c r="D2" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="I2" s="24" t="s">
+      <c r="F2" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="E16" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="7" t="s">
+      <c r="E17" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="7" t="s">
+      <c r="C27" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7" t="s">
+      <c r="D27" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E40" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D41" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="25" t="s">
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="14"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D53" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C58" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="E16" s="25" t="s">
+      <c r="D58" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="17" t="s">
+      <c r="E58" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="F58" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="G58" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="H58" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C59" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="G59" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="H59" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="I59" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H60" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I60" s="14"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G61" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F62" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="14"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="G69" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="H69" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3" t="s">
+      <c r="I69" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="H70" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I70" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I71" s="14"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="G72" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="F73" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="7" t="s">
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="25" t="s">
+      <c r="C79" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="E79" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="F79" s="29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="G36" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="3" t="s">
+      <c r="C80" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="F80" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="C49" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" s="25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E52" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="F58" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="G58" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="H58" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I58" s="25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F59" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="G59" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H59" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="I59" s="17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H60" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I60" s="3"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G61" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F62" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E63" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" s="3"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="E69" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F69" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="G69" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="H69" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="I69" s="25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F70" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="G70" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="H70" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I70" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="17"/>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72" s="3"/>
-      <c r="G72" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="F73" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="C79" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E79" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="F79" s="25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C82" s="3"/>
-      <c r="E82" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F82" s="3"/>
+      <c r="C82" s="14"/>
+      <c r="E82" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="39">

</xml_diff>

<commit_message>
updated lexicon and EOD
</commit_message>
<xml_diff>
--- a/src/main/docs/Queries_CCG_Derivation.xlsx
+++ b/src/main/docs/Queries_CCG_Derivation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="197">
   <si>
     <t xml:space="preserve">events</t>
   </si>
@@ -325,6 +325,12 @@
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">(NP/NP)/O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
   </si>
   <si>
     <t xml:space="preserve">Filter</t>
@@ -1862,7 +1868,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1888,6 +1894,7 @@
       <sz val="10.5"/>
       <name val="Source Code Pro"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
@@ -1895,11 +1902,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -2141,27 +2143,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2185,7 +2187,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2281,9 +2283,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2300,19 +2299,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:P177"/>
+  <dimension ref="A2:P201"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A159" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D168" activeCellId="0" sqref="D168"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D196" activeCellId="0" sqref="D196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.7602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7755102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
   </cols>
   <sheetData>
     <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2343,12 +2340,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+    </row>
     <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
@@ -2356,6 +2360,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
+      <c r="E6" s="0"/>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
@@ -2365,8 +2370,18 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+    </row>
+    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+    </row>
     <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -2377,6 +2392,7 @@
       <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E10" s="0"/>
     </row>
     <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
@@ -2388,14 +2404,21 @@
       <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E11" s="0"/>
+    </row>
+    <row r="12" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+    </row>
     <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4"/>
+      <c r="E13" s="0"/>
     </row>
     <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
@@ -2403,9 +2426,20 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-    </row>
-    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E14" s="0"/>
+    </row>
+    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="0"/>
+    </row>
+    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="0"/>
+    </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
         <v>10</v>
@@ -2516,8 +2550,26 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+      <c r="G24" s="0"/>
+      <c r="H24" s="0"/>
+      <c r="I24" s="0"/>
+    </row>
+    <row r="25" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
+      <c r="I25" s="0"/>
+    </row>
     <row r="26" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
         <v>0</v>
@@ -2579,11 +2631,16 @@
         <v>4</v>
       </c>
       <c r="F27" s="5"/>
+      <c r="G27" s="0"/>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
+      <c r="O27" s="0"/>
+      <c r="P27" s="0"/>
     </row>
     <row r="28" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="5"/>
@@ -2591,7 +2648,16 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="I28" s="0"/>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+      <c r="M28" s="0"/>
       <c r="N28" s="5"/>
+      <c r="O28" s="0"/>
+      <c r="P28" s="0"/>
     </row>
     <row r="29" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="3" t="s">
@@ -2600,6 +2666,17 @@
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
+      <c r="M29" s="0"/>
+      <c r="N29" s="0"/>
+      <c r="O29" s="0"/>
+      <c r="P29" s="0"/>
     </row>
     <row r="30" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
@@ -2608,6 +2685,17 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
+      <c r="M30" s="0"/>
+      <c r="N30" s="0"/>
+      <c r="O30" s="0"/>
+      <c r="P30" s="0"/>
     </row>
     <row r="31" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="3" t="s">
@@ -2616,9 +2704,52 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-    </row>
-    <row r="32" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+      <c r="M31" s="0"/>
+      <c r="N31" s="0"/>
+      <c r="O31" s="0"/>
+      <c r="P31" s="0"/>
+    </row>
+    <row r="32" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
+      <c r="M32" s="0"/>
+      <c r="N32" s="0"/>
+      <c r="O32" s="0"/>
+      <c r="P32" s="0"/>
+    </row>
+    <row r="33" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0"/>
+      <c r="L33" s="0"/>
+      <c r="M33" s="0"/>
+      <c r="N33" s="0"/>
+      <c r="O33" s="0"/>
+      <c r="P33" s="0"/>
+    </row>
     <row r="34" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="2" t="s">
         <v>0</v>
@@ -2638,6 +2769,15 @@
       <c r="G34" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
+      <c r="N34" s="0"/>
+      <c r="O34" s="0"/>
+      <c r="P34" s="0"/>
     </row>
     <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="2" t="s">
@@ -2658,9 +2798,35 @@
       <c r="G35" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
+      <c r="M35" s="0"/>
+      <c r="N35" s="0"/>
+      <c r="O35" s="0"/>
+      <c r="P35" s="0"/>
+    </row>
+    <row r="36" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
+      <c r="J36" s="0"/>
+      <c r="K36" s="0"/>
+      <c r="L36" s="0"/>
+      <c r="M36" s="0"/>
+      <c r="N36" s="0"/>
+      <c r="O36" s="0"/>
+      <c r="P36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1"/>
       <c r="B37" s="3" t="s">
         <v>4</v>
       </c>
@@ -2670,7 +2836,8 @@
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1"/>
       <c r="B38" s="3" t="s">
         <v>29</v>
       </c>
@@ -2680,7 +2847,8 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1"/>
       <c r="B39" s="3" t="s">
         <v>30</v>
       </c>
@@ -2690,7 +2858,8 @@
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
     </row>
-    <row r="40" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -2700,7 +2869,8 @@
       </c>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1"/>
       <c r="B41" s="3" t="s">
         <v>9</v>
       </c>
@@ -3177,49 +3347,49 @@
       <c r="I105" s="17"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G106" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H106" s="18"/>
-      <c r="I106" s="18"/>
+      <c r="G106" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H106" s="17"/>
+      <c r="I106" s="17"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F107" s="19" t="s">
+      <c r="F107" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G107" s="19"/>
-      <c r="H107" s="19"/>
-      <c r="I107" s="19"/>
+      <c r="G107" s="18"/>
+      <c r="H107" s="18"/>
+      <c r="I107" s="18"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E108" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F108" s="19"/>
-      <c r="G108" s="19"/>
-      <c r="H108" s="19"/>
-      <c r="I108" s="19"/>
+      <c r="E108" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
+      <c r="I108" s="18"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D109" s="19" t="s">
+      <c r="D109" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E109" s="19"/>
-      <c r="F109" s="19"/>
-      <c r="G109" s="19"/>
-      <c r="H109" s="19"/>
-      <c r="I109" s="19"/>
+      <c r="E109" s="18"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="18"/>
+      <c r="H109" s="18"/>
+      <c r="I109" s="18"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C110" s="19" t="s">
+      <c r="C110" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19"/>
-      <c r="F110" s="19"/>
-      <c r="G110" s="19"/>
-      <c r="H110" s="19"/>
-      <c r="I110" s="19"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="18"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="18"/>
+      <c r="I110" s="18"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="2" t="s">
@@ -3618,63 +3788,271 @@
       <c r="G171" s="3"/>
     </row>
     <row r="174" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="0" t="s">
+      <c r="B174" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C174" s="0" t="s">
+      <c r="C174" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D174" s="0" t="s">
+      <c r="D174" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E174" s="0" t="s">
+      <c r="E174" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F174" s="0" t="s">
+      <c r="F174" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G174" s="0" t="s">
+      <c r="G174" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H174" s="0" t="s">
+      <c r="H174" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B175" s="7" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C175" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E175" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F175" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G175" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H175" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C177" s="19"/>
+      <c r="G177" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H177" s="3"/>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F178" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G178" s="3"/>
+      <c r="H178" s="3"/>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E179" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F179" s="14"/>
+      <c r="G179" s="14"/>
+      <c r="H179" s="14"/>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D180" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E180" s="14"/>
+      <c r="F180" s="14"/>
+      <c r="G180" s="14"/>
+      <c r="H180" s="14"/>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C181" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D181" s="14"/>
+      <c r="E181" s="14"/>
+      <c r="F181" s="14"/>
+      <c r="G181" s="14"/>
+      <c r="H181" s="14"/>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B182" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C182" s="14"/>
+      <c r="D182" s="14"/>
+      <c r="E182" s="14"/>
+      <c r="F182" s="14"/>
+      <c r="G182" s="14"/>
+      <c r="H182" s="14"/>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B186" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B187" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C187" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D187" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D175" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F175" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="G175" s="0" t="s">
+      <c r="E187" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B188" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C188" s="14"/>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B189" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C189" s="14"/>
+      <c r="D189" s="14"/>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B190" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C190" s="14"/>
+      <c r="D190" s="14"/>
+      <c r="E190" s="14"/>
+    </row>
+    <row r="193" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B193" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F193" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B194" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C194" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H175" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G176" s="19" t="s">
+      <c r="D194" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E194" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F194" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B195" s="12"/>
+      <c r="C195" s="20"/>
+      <c r="D195" s="20"/>
+      <c r="E195" s="20"/>
+      <c r="F195" s="20"/>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D196" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E196" s="14"/>
+      <c r="F196" s="14"/>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C197" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H176" s="19"/>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F177" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G177" s="19"/>
-      <c r="H177" s="19"/>
+      <c r="D197" s="14"/>
+      <c r="E197" s="14"/>
+      <c r="F197" s="14"/>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B198" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C198" s="14"/>
+      <c r="D198" s="14"/>
+      <c r="E198" s="14"/>
+      <c r="F198" s="14"/>
+    </row>
+    <row r="200" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B200" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E200" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F200" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G200" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H200" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I200" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B201" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C201" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D201" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E201" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F201" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G201" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H201" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I201" s="7" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="76">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:E7"/>
@@ -3739,8 +4117,18 @@
     <mergeCell ref="E169:G169"/>
     <mergeCell ref="D170:G170"/>
     <mergeCell ref="B171:G171"/>
-    <mergeCell ref="G176:H176"/>
-    <mergeCell ref="F177:H177"/>
+    <mergeCell ref="G177:H177"/>
+    <mergeCell ref="F178:H178"/>
+    <mergeCell ref="E179:H179"/>
+    <mergeCell ref="D180:H180"/>
+    <mergeCell ref="C181:H181"/>
+    <mergeCell ref="B182:H182"/>
+    <mergeCell ref="B188:C188"/>
+    <mergeCell ref="B189:D189"/>
+    <mergeCell ref="B190:E190"/>
+    <mergeCell ref="D196:F196"/>
+    <mergeCell ref="C197:F197"/>
+    <mergeCell ref="B198:F198"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3765,24 +4153,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.8163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="87.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="20" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="20" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="20" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="20" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="85.9897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="20" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="20" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="20" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="20" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="21"/>
       <c r="D1" s="21"/>
       <c r="G1" s="22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
@@ -3794,37 +4178,37 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3832,19 +4216,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K4" s="20" t="s">
         <v>12</v>
@@ -3852,19 +4236,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>82</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>80</v>
       </c>
       <c r="G5" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K5" s="20" t="s">
         <v>12</v>
@@ -3872,44 +4256,44 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K8" s="20" t="s">
         <v>12</v>
@@ -3917,70 +4301,70 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>12</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>12</v>
@@ -3988,158 +4372,158 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="N23" s="20" t="s">
         <v>19</v>
@@ -4147,189 +4531,189 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K24" s="20" t="s">
         <v>44</v>
       </c>
       <c r="L24" s="20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>12</v>
       </c>
       <c r="L26" s="20" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>12</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>12</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>12</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="M31" s="20" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="24" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D39" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4359,13 +4743,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="259.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -4391,9 +4772,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4418,10 +4796,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4432,19 +4808,19 @@
         <v>11</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I2" s="28" t="s">
         <v>44</v>
@@ -4463,7 +4839,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>28</v>
@@ -4472,10 +4848,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>28</v>
@@ -4502,7 +4878,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -4536,7 +4912,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -4565,13 +4941,13 @@
         <v>11</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4579,16 +4955,16 @@
         <v>14</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4606,7 +4982,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="14" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -4623,13 +4999,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E27" s="29" t="s">
         <v>44</v>
@@ -4637,10 +5013,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>28</v>
@@ -4663,7 +5039,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -4690,10 +5066,10 @@
         <v>13</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4701,7 +5077,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>28</v>
@@ -4710,10 +5086,10 @@
         <v>28</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4739,7 +5115,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="14" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
@@ -4758,19 +5134,19 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="29" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E49" s="29" t="s">
         <v>13</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4784,10 +5160,10 @@
         <v>28</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4831,19 +5207,19 @@
         <v>13</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F58" s="29" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G58" s="29" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H58" s="29" t="s">
         <v>13</v>
       </c>
       <c r="I58" s="29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4860,16 +5236,16 @@
         <v>4</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G59" s="20" t="s">
         <v>28</v>
       </c>
       <c r="H59" s="20" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I59" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4887,7 +5263,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F62" s="14" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G62" s="14"/>
       <c r="H62" s="14"/>
@@ -4895,7 +5271,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="14" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
@@ -4935,19 +5311,19 @@
         <v>11</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E69" s="29" t="s">
         <v>13</v>
       </c>
       <c r="F69" s="29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G69" s="29" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H69" s="29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I69" s="29" t="s">
         <v>44</v>
@@ -4967,10 +5343,10 @@
         <v>5</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G70" s="20" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H70" s="20" t="s">
         <v>28</v>
@@ -4997,7 +5373,7 @@
       </c>
       <c r="C72" s="14"/>
       <c r="G72" s="14" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
@@ -5037,30 +5413,30 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C79" s="29" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E79" s="29" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F79" s="29" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="12" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated lexicon for all the events and other lexicons - DateAndLocation added
</commit_message>
<xml_diff>
--- a/src/main/docs/Queries_CCG_Derivation.xlsx
+++ b/src/main/docs/Queries_CCG_Derivation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="205">
   <si>
     <t xml:space="preserve">events</t>
   </si>
@@ -331,6 +331,30 @@
   </si>
   <si>
     <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NP/V)\NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NP/NP)/V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(S\O)\NP)/NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NP\O)\NP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(NP\O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(S\O)/NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(S\O)</t>
   </si>
   <si>
     <t xml:space="preserve">Filter</t>
@@ -1868,7 +1892,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1902,6 +1926,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -2078,7 +2107,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2167,6 +2196,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2187,7 +2232,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2299,14 +2344,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:P201"/>
+  <dimension ref="A2:P238"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D196" activeCellId="0" sqref="D196"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C226" activeCellId="0" sqref="C226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7755102040816"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7755102040816"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
@@ -3999,60 +4045,307 @@
       <c r="E198" s="14"/>
       <c r="F198" s="14"/>
     </row>
-    <row r="200" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B200" s="2" t="s">
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B201" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C201" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D201" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E201" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F201" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B202" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D202" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E202" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F202" s="22"/>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B203" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C203" s="23"/>
+    </row>
+    <row r="207" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B207" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C200" s="2" t="s">
+      <c r="C207" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D200" s="2" t="s">
+      <c r="D207" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E200" s="2" t="s">
+      <c r="E207" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F200" s="2" t="s">
+      <c r="F207" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G200" s="2" t="s">
+      <c r="G207" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H200" s="2" t="s">
+      <c r="H207" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I200" s="2" t="s">
+      <c r="I207" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B201" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C201" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D201" s="7" t="s">
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B208" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C208" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D208" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E208" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F208" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E201" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F201" s="7" t="s">
+      <c r="G208" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H208" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G201" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H201" s="7" t="s">
+      <c r="I208" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G210" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H210" s="14"/>
+      <c r="I210" s="14"/>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F211" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G211" s="14"/>
+      <c r="H211" s="14"/>
+      <c r="I211" s="14"/>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E212" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F212" s="14"/>
+      <c r="G212" s="14"/>
+      <c r="H212" s="14"/>
+      <c r="I212" s="14"/>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D213" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E213" s="24"/>
+      <c r="F213" s="24"/>
+      <c r="G213" s="24"/>
+      <c r="H213" s="24"/>
+      <c r="I213" s="24"/>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C214" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D214" s="14"/>
+      <c r="E214" s="14"/>
+      <c r="F214" s="14"/>
+      <c r="G214" s="14"/>
+      <c r="H214" s="14"/>
+      <c r="I214" s="14"/>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B215" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C215" s="14"/>
+      <c r="D215" s="14"/>
+      <c r="E215" s="14"/>
+      <c r="F215" s="14"/>
+      <c r="G215" s="14"/>
+      <c r="H215" s="14"/>
+      <c r="I215" s="14"/>
+    </row>
+    <row r="219" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C219" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E219" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F219" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G219" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H219" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I219" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C220" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D220" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E220" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F220" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I201" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="G220" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H220" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I220" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G222" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H222" s="14"/>
+      <c r="I222" s="14"/>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F223" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G223" s="14"/>
+      <c r="H223" s="14"/>
+      <c r="I223" s="14"/>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E224" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F224" s="14"/>
+      <c r="G224" s="14"/>
+      <c r="H224" s="14"/>
+      <c r="I224" s="14"/>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D225" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E225" s="24"/>
+      <c r="F225" s="24"/>
+      <c r="G225" s="24"/>
+      <c r="H225" s="24"/>
+      <c r="I225" s="24"/>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C226" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D226" s="14"/>
+      <c r="E226" s="14"/>
+      <c r="F226" s="14"/>
+      <c r="G226" s="14"/>
+      <c r="H226" s="14"/>
+      <c r="I226" s="14"/>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B233" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E233" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F233" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G233" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B234" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C234" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D234" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E234" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F234" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G234" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F236" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G236" s="22"/>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E237" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F237" s="22"/>
+      <c r="G237" s="22"/>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D238" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E238" s="22"/>
+      <c r="F238" s="22"/>
+      <c r="G238" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="76">
+  <mergeCells count="92">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:E7"/>
@@ -4129,6 +4422,22 @@
     <mergeCell ref="D196:F196"/>
     <mergeCell ref="C197:F197"/>
     <mergeCell ref="B198:F198"/>
+    <mergeCell ref="E202:F202"/>
+    <mergeCell ref="B203:C203"/>
+    <mergeCell ref="G210:I210"/>
+    <mergeCell ref="F211:I211"/>
+    <mergeCell ref="E212:I212"/>
+    <mergeCell ref="D213:I213"/>
+    <mergeCell ref="C214:I214"/>
+    <mergeCell ref="B215:I215"/>
+    <mergeCell ref="G222:I222"/>
+    <mergeCell ref="F223:I223"/>
+    <mergeCell ref="E224:I224"/>
+    <mergeCell ref="D225:I225"/>
+    <mergeCell ref="C226:I226"/>
+    <mergeCell ref="F236:G236"/>
+    <mergeCell ref="E237:G237"/>
+    <mergeCell ref="D238:G238"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4163,72 +4472,72 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="G1" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="G1" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="N2" s="21" t="s">
+      <c r="F2" s="25" t="s">
         <v>79</v>
       </c>
+      <c r="G2" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="21"/>
+      <c r="B3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>81</v>
+        <v>88</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>89</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="K4" s="20" t="s">
         <v>12</v>
@@ -4236,64 +4545,64 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>85</v>
+        <v>92</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G5" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="K5" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="23" t="s">
-        <v>87</v>
+      <c r="D6" s="27" t="s">
+        <v>95</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="23" t="s">
-        <v>88</v>
+      <c r="D7" s="27" t="s">
+        <v>96</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>90</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>82</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="K8" s="20" t="s">
         <v>12</v>
@@ -4301,70 +4610,70 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>94</v>
+        <v>101</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>102</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>98</v>
+        <v>105</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>106</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>12</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>12</v>
@@ -4372,158 +4681,158 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>103</v>
+        <v>110</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>113</v>
+        <v>120</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>121</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>122</v>
+        <v>105</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="E20" s="26"/>
+        <v>131</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="30"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E21" s="26"/>
+        <v>133</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="L22" s="20" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="N23" s="20" t="s">
         <v>19</v>
@@ -4531,189 +4840,189 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="K24" s="20" t="s">
         <v>44</v>
       </c>
       <c r="L24" s="20" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>139</v>
+        <v>146</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>12</v>
       </c>
       <c r="L26" s="20" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>145</v>
+        <v>152</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>147</v>
+        <v>154</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>12</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>12</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>154</v>
+        <v>161</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>162</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>12</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="M31" s="20" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="24" t="s">
-        <v>160</v>
+      <c r="B33" s="28" t="s">
+        <v>168</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="0" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D39" s="0" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="0" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -4745,8 +5054,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <sheetData>
     <row r="5" customFormat="false" ht="259.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="27" t="s">
-        <v>173</v>
+      <c r="D5" s="31" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4801,45 +5110,45 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="E2" s="28" t="s">
+      <c r="D2" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>176</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>177</v>
-      </c>
-      <c r="I2" s="28" t="s">
+      <c r="F2" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="I2" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>28</v>
@@ -4848,10 +5157,10 @@
         <v>28</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>28</v>
@@ -4878,7 +5187,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -4912,7 +5221,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="3" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -4934,20 +5243,20 @@
       <c r="I11" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" s="29" t="s">
+      <c r="D16" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="E16" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="29" t="s">
-        <v>175</v>
+      <c r="F16" s="33" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4955,16 +5264,16 @@
         <v>14</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4982,7 +5291,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="14" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -4998,25 +5307,25 @@
       <c r="F22" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="E27" s="29" t="s">
+      <c r="B27" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="20" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>28</v>
@@ -5039,7 +5348,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -5053,23 +5362,23 @@
       <c r="E32" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E36" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>175</v>
+      <c r="F36" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5077,7 +5386,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>28</v>
@@ -5086,10 +5395,10 @@
         <v>28</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5115,7 +5424,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="14" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
@@ -5133,20 +5442,20 @@
       <c r="G43" s="14"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>187</v>
-      </c>
-      <c r="D49" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="E49" s="29" t="s">
+      <c r="B49" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="E49" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="29" t="s">
-        <v>189</v>
+      <c r="F49" s="33" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5160,10 +5469,10 @@
         <v>28</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5197,29 +5506,29 @@
       <c r="F55" s="14"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="29" t="s">
+      <c r="D58" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E58" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="F58" s="29" t="s">
-        <v>187</v>
-      </c>
-      <c r="G58" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="H58" s="29" t="s">
+      <c r="E58" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="F58" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="G58" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="H58" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="I58" s="29" t="s">
-        <v>189</v>
+      <c r="I58" s="33" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5236,16 +5545,16 @@
         <v>4</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G59" s="20" t="s">
         <v>28</v>
       </c>
       <c r="H59" s="20" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="I59" s="20" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5263,7 +5572,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F62" s="14" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="G62" s="14"/>
       <c r="H62" s="14"/>
@@ -5271,7 +5580,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="14" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="F63" s="14"/>
       <c r="G63" s="14"/>
@@ -5304,28 +5613,28 @@
       <c r="I66" s="14"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="29" t="s">
+      <c r="B69" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C69" s="29" t="s">
+      <c r="C69" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="E69" s="29" t="s">
+      <c r="D69" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="E69" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F69" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="G69" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="H69" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="I69" s="29" t="s">
+      <c r="F69" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="G69" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="H69" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="I69" s="33" t="s">
         <v>44</v>
       </c>
     </row>
@@ -5343,10 +5652,10 @@
         <v>5</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="G70" s="20" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="H70" s="20" t="s">
         <v>28</v>
@@ -5373,7 +5682,7 @@
       </c>
       <c r="C72" s="14"/>
       <c r="G72" s="14" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
@@ -5412,31 +5721,31 @@
       <c r="I75" s="14"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="C79" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="E79" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="F79" s="29" t="s">
-        <v>175</v>
+      <c r="B79" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="C79" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="E79" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="F79" s="33" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="12" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="F80" s="12" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>